<commit_message>
AUD ON Curve first version
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/AUD_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/AUD_MainChecks.xlsx
@@ -775,6 +775,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
+<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <volType type="realTimeData">
+    <main first="pldatasource.rdatartdserver">
+      <tp t="s">
+        <v>Updated at 17:22:31</v>
+        <stp/>
+        <stp>{0F07BAC8-C1A3-4421-B88C-394D3FA91D1E}</stp>
+        <tr r="I3" s="2"/>
+      </tp>
+    </main>
+  </volType>
+</volTypes>
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1164,9 +1179,7 @@
   </sheetPr>
   <dimension ref="A1:W58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1232,7 +1245,9 @@
       <c r="H2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="39"/>
+      <c r="I2" s="39">
+        <v>41802.723634259259</v>
+      </c>
       <c r="J2" s="13"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -1256,24 +1271,24 @@
       </c>
       <c r="C3" s="48">
         <f>_xll.qlCalendarAdjust("JAPAN",_xll.qlSettingsEvaluationDate(ISERROR(Trigger)),"f")</f>
-        <v>41796</v>
+        <v>41802</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="17" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(B3,C3,,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F3" s="18" t="e">
+        <f>_xll.qlYieldTSDiscount(B3,C3,,Trigger)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F3" s="18" t="str">
         <f ca="1">IF(ISERROR(C3),_xll.ohRangeRetrieveError(C3),_xll.ohRangeRetrieveError(E3))</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="45" t="e">
-        <f ca="1">_xll.RData(H4,"LAST",,"FRQ:1S",,I4)</f>
-        <v>#NAME?</v>
+      <c r="I3" s="45" t="str">
+        <f>_xll.RData(H4,"LAST",,"FRQ:1S",,I4)</f>
+        <v>Updated at 17:22:31</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="4"/>
@@ -1298,23 +1313,23 @@
       </c>
       <c r="C4" s="40">
         <f>EvaluationDate</f>
-        <v>41796</v>
+        <v>41802</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="17" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(B4,C4,,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F4" s="18" t="e">
+        <f>_xll.qlYieldTSDiscount(B4,C4,,Trigger)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F4" s="18" t="str">
         <f ca="1">IF(ISERROR(C4),_xll.ohRangeRetrieveError(C4),_xll.ohRangeRetrieveError(E4))</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="47" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="44">
-        <v>146.6</v>
+        <v>145.26</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="4"/>
@@ -1338,17 +1353,17 @@
         <v>AUD3M</v>
       </c>
       <c r="C5" s="40" t="e">
-        <f ca="1">_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
-        <v>#NAME?</v>
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="17" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(B5,C5,,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F5" s="18" t="e">
+        <f>_xll.qlYieldTSDiscount(B5,C5,,Trigger)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F5" s="18" t="str">
         <f ca="1">IF(ISERROR(C5),_xll.ohRangeRetrieveError(C5),_xll.ohRangeRetrieveError(E5))</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="19" t="s">
@@ -1356,7 +1371,7 @@
       </c>
       <c r="I5" s="20">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>851</v>
+        <v>35</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="4"/>
@@ -1380,17 +1395,17 @@
         <v>AUD6M</v>
       </c>
       <c r="C6" s="40" t="e">
-        <f ca="1">_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
-        <v>#NAME?</v>
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="17" t="e">
-        <f ca="1">_xll.qlYieldTSDiscount(B6,C6,,Trigger)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F6" s="18" t="e">
+        <f>_xll.qlYieldTSDiscount(B6,C6,,Trigger)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F6" s="18" t="str">
         <f ca="1">IF(ISERROR(C6),_xll.ohRangeRetrieveError(C6),_xll.ohRangeRetrieveError(E6))</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="33" t="s">
@@ -1418,17 +1433,17 @@
       <c r="A7" s="6"/>
       <c r="B7" s="23"/>
       <c r="C7" s="41" t="e">
-        <f ca="1">_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
-        <v>#NAME?</v>
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25" t="e">
-        <f ca="1">_xll.qlIndexFixing(FirstIndex,C7)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F7" s="14" t="e">
+        <f>_xll.qlIndexFixing(FirstIndex,C7)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F7" s="14" t="str">
         <f ca="1">IF(ISERROR(C7),_xll.ohRangeRetrieveError(C7),_xll.ohRangeRetrieveError(E7))</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="21" t="s">
@@ -1457,17 +1472,17 @@
       <c r="A8" s="6"/>
       <c r="B8" s="26"/>
       <c r="C8" s="42" t="e">
-        <f ca="1">_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
-        <v>#NAME?</v>
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D8" s="35"/>
       <c r="E8" s="28" t="e">
-        <f ca="1">_xll.qlIndexFixing(FirstIndex,C8)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F8" s="18" t="e">
+        <f>_xll.qlIndexFixing(FirstIndex,C8)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F8" s="18" t="str">
         <f ca="1">IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(E8))</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="21" t="s">
@@ -1500,16 +1515,16 @@
       </c>
       <c r="C9" s="42">
         <f>EvaluationDate</f>
-        <v>41796</v>
+        <v>41802</v>
       </c>
       <c r="D9" s="27"/>
       <c r="E9" s="28" t="e">
-        <f ca="1">_xll.qlIndexFixing(FirstIndex,C9)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F9" s="18" t="e">
+        <f>_xll.qlIndexFixing(FirstIndex,C9)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F9" s="18" t="str">
         <f ca="1">IF(ISERROR(C9),_xll.ohRangeRetrieveError(C9),_xll.ohRangeRetrieveError(E9))</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G9" s="11"/>
       <c r="H9" s="33" t="s">
@@ -1538,17 +1553,17 @@
       <c r="A10" s="6"/>
       <c r="B10" s="29"/>
       <c r="C10" s="43" t="e">
-        <f ca="1">_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlIMMNextDate(_xll.qlIMMNextDate(EvaluationDate+1)+1),-_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
-        <v>#NAME?</v>
+        <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlIMMNextDate(_xll.qlIMMNextDate(EvaluationDate+1)+1),-_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" s="31" t="e">
-        <f ca="1">_xll.qlIndexFixing(FirstIndex,C10,TRUE)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F10" s="32" t="e">
+        <f>_xll.qlIndexFixing(FirstIndex,C10,TRUE)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="F10" s="32" t="str">
         <f ca="1">IF(ISERROR(C10),_xll.ohRangeRetrieveError(C10),_xll.ohRangeRetrieveError(E10))</f>
-        <v>#NAME?</v>
+        <v/>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="50"/>
@@ -2710,6 +2725,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+      <formula1>"EUR,USD,GBP,JPY,CHF,AUD"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="33" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -2718,7 +2738,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="CommandButton1">
+        <control shapeId="1026" r:id="rId4" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -2738,12 +2758,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="CommandButton2">
+        <control shapeId="1025" r:id="rId6" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -2763,7 +2783,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
AUD 3M curve first version
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/AUD_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/AUD_MainChecks.xlsx
@@ -782,9 +782,9 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 17:22:31</v>
+        <v>Updated at 18:16:21</v>
         <stp/>
-        <stp>{0F07BAC8-C1A3-4421-B88C-394D3FA91D1E}</stp>
+        <stp>{D06E9DEB-050F-4358-9B5B-301044FB4292}</stp>
         <tr r="I3" s="2"/>
       </tp>
     </main>
@@ -1179,7 +1179,9 @@
   </sheetPr>
   <dimension ref="A1:W58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1245,9 +1247,7 @@
       <c r="H2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="39">
-        <v>41802.723634259259</v>
-      </c>
+      <c r="I2" s="39"/>
       <c r="J2" s="13"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="C3" s="48">
         <f>_xll.qlCalendarAdjust("JAPAN",_xll.qlSettingsEvaluationDate(ISERROR(Trigger)),"f")</f>
-        <v>41802</v>
+        <v>41806</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="17" t="e">
@@ -1280,7 +1280,7 @@
       </c>
       <c r="F3" s="18" t="str">
         <f ca="1">IF(ISERROR(C3),_xll.ohRangeRetrieveError(C3),_xll.ohRangeRetrieveError(E3))</f>
-        <v/>
+        <v>qlYieldTSDiscount - ObjectHandler error: attempt to retrieve object with unknown ID 'AUDSTD'</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="46" t="s">
@@ -1288,7 +1288,7 @@
       </c>
       <c r="I3" s="45" t="str">
         <f>_xll.RData(H4,"LAST",,"FRQ:1S",,I4)</f>
-        <v>Updated at 17:22:31</v>
+        <v>Updated at 18:16:21</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="4"/>
@@ -1313,15 +1313,15 @@
       </c>
       <c r="C4" s="40">
         <f>EvaluationDate</f>
-        <v>41802</v>
+        <v>41806</v>
       </c>
       <c r="D4" s="16"/>
-      <c r="E4" s="17" t="e">
+      <c r="E4" s="17">
         <f>_xll.qlYieldTSDiscount(B4,C4,,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="F4" s="18" t="str">
-        <f ca="1">IF(ISERROR(C4),_xll.ohRangeRetrieveError(C4),_xll.ohRangeRetrieveError(E4))</f>
+        <f>IF(ISERROR(C4),_xll.ohRangeRetrieveError(C4),_xll.ohRangeRetrieveError(E4))</f>
         <v/>
       </c>
       <c r="G4" s="11"/>
@@ -1329,7 +1329,7 @@
         <v>12</v>
       </c>
       <c r="I4" s="44">
-        <v>145.26</v>
+        <v>145.66</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="4"/>
@@ -1352,17 +1352,17 @@
         <f>UPPER(Currency)&amp;"3M"</f>
         <v>AUD3M</v>
       </c>
-      <c r="C5" s="40" t="e">
+      <c r="C5" s="40">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
-        <v>#VALUE!</v>
+        <v>41806</v>
       </c>
       <c r="D5" s="16"/>
-      <c r="E5" s="17" t="e">
+      <c r="E5" s="17">
         <f>_xll.qlYieldTSDiscount(B5,C5,,Trigger)</f>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="F5" s="18" t="str">
-        <f ca="1">IF(ISERROR(C5),_xll.ohRangeRetrieveError(C5),_xll.ohRangeRetrieveError(E5))</f>
+        <f>IF(ISERROR(C5),_xll.ohRangeRetrieveError(C5),_xll.ohRangeRetrieveError(E5))</f>
         <v/>
       </c>
       <c r="G5" s="11"/>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="I5" s="20">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>35</v>
+        <v>513</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="4"/>
@@ -1394,9 +1394,9 @@
         <f>UPPER(Currency)&amp;"6M"</f>
         <v>AUD6M</v>
       </c>
-      <c r="C6" s="40" t="e">
+      <c r="C6" s="40">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
-        <v>#VALUE!</v>
+        <v>41806</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="17" t="e">
@@ -1405,7 +1405,7 @@
       </c>
       <c r="F6" s="18" t="str">
         <f ca="1">IF(ISERROR(C6),_xll.ohRangeRetrieveError(C6),_xll.ohRangeRetrieveError(E6))</f>
-        <v/>
+        <v>qlYieldTSDiscount - empty Handle cannot be dereferenced</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="33" t="s">
@@ -1432,9 +1432,9 @@
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="23"/>
-      <c r="C7" s="41" t="e">
+      <c r="C7" s="41">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
-        <v>#VALUE!</v>
+        <v>41802</v>
       </c>
       <c r="D7" s="24"/>
       <c r="E7" s="25" t="e">
@@ -1443,7 +1443,7 @@
       </c>
       <c r="F7" s="14" t="str">
         <f ca="1">IF(ISERROR(C7),_xll.ohRangeRetrieveError(C7),_xll.ohRangeRetrieveError(E7))</f>
-        <v/>
+        <v>qlIndexFixing - Missing BBSW6M Actual/365 (Fixed) fixing for June 12th, 2014</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="21" t="s">
@@ -1471,9 +1471,9 @@
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
       <c r="B8" s="26"/>
-      <c r="C8" s="42" t="e">
+      <c r="C8" s="42">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
-        <v>#VALUE!</v>
+        <v>41803</v>
       </c>
       <c r="D8" s="35"/>
       <c r="E8" s="28" t="e">
@@ -1482,7 +1482,7 @@
       </c>
       <c r="F8" s="18" t="str">
         <f ca="1">IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(E8))</f>
-        <v/>
+        <v>qlIndexFixing - Missing BBSW6M Actual/365 (Fixed) fixing for June 13th, 2014</v>
       </c>
       <c r="G8" s="11"/>
       <c r="H8" s="21" t="s">
@@ -1510,20 +1510,20 @@
     <row r="9" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="26" t="str">
-        <f>PROPER(Currency)&amp;IF(UPPER(Currency)="EUR","",IF(UPPER(Currency)="HKD","H","L"))&amp;"ibor6M"</f>
-        <v>AudLibor6M</v>
+        <f>PROPER(Currency)&amp;"BBSW"&amp;"6M"</f>
+        <v>AudBBSW6M</v>
       </c>
       <c r="C9" s="42">
         <f>EvaluationDate</f>
-        <v>41802</v>
+        <v>41806</v>
       </c>
       <c r="D9" s="27"/>
-      <c r="E9" s="28" t="e">
+      <c r="E9" s="28">
         <f>_xll.qlIndexFixing(FirstIndex,C9)</f>
-        <v>#NUM!</v>
+        <v>2.7099999999999999E-2</v>
       </c>
       <c r="F9" s="18" t="str">
-        <f ca="1">IF(ISERROR(C9),_xll.ohRangeRetrieveError(C9),_xll.ohRangeRetrieveError(E9))</f>
+        <f>IF(ISERROR(C9),_xll.ohRangeRetrieveError(C9),_xll.ohRangeRetrieveError(E9))</f>
         <v/>
       </c>
       <c r="G9" s="11"/>
@@ -1552,9 +1552,9 @@
     <row r="10" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="29"/>
-      <c r="C10" s="43" t="e">
+      <c r="C10" s="43">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlIMMNextDate(_xll.qlIMMNextDate(EvaluationDate+1)+1),-_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
-        <v>#VALUE!</v>
+        <v>41899</v>
       </c>
       <c r="D10" s="30"/>
       <c r="E10" s="31" t="e">
@@ -1563,7 +1563,7 @@
       </c>
       <c r="F10" s="32" t="str">
         <f ca="1">IF(ISERROR(C10),_xll.ohRangeRetrieveError(C10),_xll.ohRangeRetrieveError(E10))</f>
-        <v/>
+        <v>qlIndexFixing - null term structure set to this instance of BBSW6M Actual/365 (Fixed)</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="50"/>
@@ -2738,7 +2738,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="CommandButton2">
+        <control shapeId="1025" r:id="rId4" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -2758,12 +2758,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="CommandButton1">
+        <control shapeId="1026" r:id="rId6" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -2783,7 +2783,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Fixing evaluation date in Main Checks
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/AUD_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/AUD_MainChecks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15285" yWindow="-15" windowWidth="15330" windowHeight="8640"/>
+    <workbookView xWindow="9585" yWindow="-15" windowWidth="9630" windowHeight="12015"/>
   </bookViews>
   <sheets>
     <sheet name="MainChecks" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <definedName name="FirstIndex">MainChecks!$B$7</definedName>
     <definedName name="InterestRatesTrigger">MainChecks!#REF!</definedName>
     <definedName name="SecondIMMDate">MainChecks!$C$10</definedName>
-    <definedName name="Trigger">MainChecks!$I$2</definedName>
+    <definedName name="Trigger">MainChecks!$H$2</definedName>
     <definedName name="Yesterday">MainChecks!$C$7</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -71,7 +71,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="9">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.0000%"/>
@@ -79,7 +79,6 @@
     <numFmt numFmtId="168" formatCode="#,##0.0;#,##0.0"/>
     <numFmt numFmtId="169" formatCode="General_)"/>
     <numFmt numFmtId="170" formatCode="ddd\,\ dd\-mmm\-yyyy\,\ hh:mm:ss"/>
-    <numFmt numFmtId="171" formatCode="ddd\,\ d\-mmm\-yyyy"/>
     <numFmt numFmtId="172" formatCode="yyyy\-mmm\-dd\-hh:mm:ss"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
@@ -598,7 +597,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -609,9 +608,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -625,9 +621,6 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="8" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -644,19 +637,10 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="6" fillId="5" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="6" fillId="5" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="6" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="5" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -667,9 +651,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="6" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -718,6 +699,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="1"/>
@@ -812,10 +794,10 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 11:41:53</v>
+        <v>Updated at 09:20:46</v>
         <stp/>
-        <stp>{236BF330-2243-41BA-B3DB-471CD82524CE}</stp>
-        <tr r="I3" s="2"/>
+        <stp>{B29BF177-39B7-4281-B10F-4A7C05F60892}</stp>
+        <tr r="H3" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1207,10 +1189,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W58"/>
+  <dimension ref="A1:V58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1218,17 +1200,16 @@
     <col min="1" max="1" width="2.7109375" style="5" customWidth="1"/>
     <col min="2" max="2" width="10" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="5" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.7109375" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="4" max="4" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>13</v>
@@ -1242,8 +1223,8 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -1256,29 +1237,28 @@
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-    </row>
-    <row r="2" spans="1:23" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="8" t="s">
+        <v>1</v>
+      </c>
       <c r="E2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="12" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="13"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -1291,36 +1271,35 @@
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-    </row>
-    <row r="3" spans="1:23" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
-      <c r="B3" s="15" t="str">
+      <c r="B3" s="14" t="str">
         <f>UPPER(Currency)&amp;"STD"</f>
         <v>AUDSTD</v>
       </c>
-      <c r="C3" s="45">
-        <f>_xll.qlCalendarAdjust("JAPAN",_xll.qlSettingsEvaluationDate(ISERROR(Trigger)),"f")</f>
-        <v>41820</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17">
+      <c r="C3" s="39">
+        <f>_xll.qlCalendarAdjust("Australia",_xll.qlSettingsEvaluationDate(ISERROR(Trigger)),"f")</f>
+        <v>41822</v>
+      </c>
+      <c r="D3" s="15">
         <f>_xll.qlYieldTSDiscount(B3,C3,,Trigger)</f>
         <v>1</v>
       </c>
-      <c r="F3" s="18" t="str">
-        <f>IF(ISERROR(C3),_xll.ohRangeRetrieveError(C3),_xll.ohRangeRetrieveError(E3))</f>
+      <c r="E3" s="16" t="str">
+        <f>IF(ISERROR(C3),_xll.ohRangeRetrieveError(C3),_xll.ohRangeRetrieveError(D3))</f>
         <v/>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="43" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="42" t="str">
-        <f>_xll.RData(H4,"LAST",,"FRQ:1S",,I4)</f>
-        <v>Updated at 11:41:53</v>
-      </c>
-      <c r="J3" s="13"/>
+      <c r="H3" s="36" t="str">
+        <f>_xll.RData(G4,"LAST",,"FRQ:1S",,H4)</f>
+        <v>Updated at 09:20:46</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="4"/>
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -1333,35 +1312,34 @@
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-    </row>
-    <row r="4" spans="1:23" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
-      <c r="B4" s="15" t="str">
+      <c r="B4" s="14" t="str">
         <f>UPPER(Currency)&amp;"ON"</f>
         <v>AUDON</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="31">
         <f>EvaluationDate</f>
-        <v>41820</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="17">
+        <v>41822</v>
+      </c>
+      <c r="D4" s="15">
         <f>_xll.qlYieldTSDiscount(B4,C4,,Trigger)</f>
         <v>1</v>
       </c>
-      <c r="F4" s="18" t="str">
-        <f>IF(ISERROR(C4),_xll.ohRangeRetrieveError(C4),_xll.ohRangeRetrieveError(E4))</f>
+      <c r="E4" s="16" t="str">
+        <f>IF(ISERROR(C4),_xll.ohRangeRetrieveError(C4),_xll.ohRangeRetrieveError(D4))</f>
         <v/>
       </c>
-      <c r="G4" s="11"/>
-      <c r="H4" s="44" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="41">
-        <v>147.03</v>
-      </c>
-      <c r="J4" s="13"/>
+      <c r="H4" s="35">
+        <v>147.04</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
@@ -1374,36 +1352,35 @@
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-    </row>
-    <row r="5" spans="1:23" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
-      <c r="B5" s="15" t="str">
+      <c r="B5" s="14" t="str">
         <f>UPPER(Currency)&amp;"3M"</f>
         <v>AUD3M</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="31">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
-        <v>41820</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17">
+        <v>41822</v>
+      </c>
+      <c r="D5" s="15">
         <f>_xll.qlYieldTSDiscount(B5,C5,,Trigger)</f>
         <v>1</v>
       </c>
-      <c r="F5" s="18" t="str">
-        <f>IF(ISERROR(C5),_xll.ohRangeRetrieveError(C5),_xll.ohRangeRetrieveError(E5))</f>
+      <c r="E5" s="16" t="str">
+        <f>IF(ISERROR(C5),_xll.ohRangeRetrieveError(C5),_xll.ohRangeRetrieveError(D5))</f>
         <v/>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="19" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="20">
+      <c r="H5" s="18">
         <f>_xll.ohRepositoryObjectCount(Trigger)</f>
         <v>775</v>
       </c>
-      <c r="J5" s="13"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
@@ -1416,35 +1393,34 @@
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-    </row>
-    <row r="6" spans="1:23" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="15" t="str">
+      <c r="B6" s="14" t="str">
         <f>UPPER(Currency)&amp;"6M"</f>
         <v>AUD6M</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="31">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
-        <v>41820</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17">
+        <v>41822</v>
+      </c>
+      <c r="D6" s="15">
         <f>_xll.qlYieldTSDiscount(B6,C6,,Trigger)</f>
         <v>1</v>
       </c>
-      <c r="F6" s="18" t="str">
-        <f>IF(ISERROR(C6),_xll.ohRangeRetrieveError(C6),_xll.ohRangeRetrieveError(E6))</f>
+      <c r="E6" s="16" t="str">
+        <f>IF(ISERROR(C6),_xll.ohRangeRetrieveError(C6),_xll.ohRangeRetrieveError(D6))</f>
         <v/>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="30" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="H6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="13"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
@@ -1457,36 +1433,35 @@
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-    </row>
-    <row r="7" spans="1:23" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
-      <c r="B7" s="48" t="str">
+      <c r="B7" s="42" t="str">
         <f>PROPER(Currency)&amp;"BBSW"&amp;"6M"</f>
         <v>AudBBSW6M</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="32">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-2D","Preceding")</f>
-        <v>41816</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24" t="e">
+        <v>41820</v>
+      </c>
+      <c r="D7" s="21" t="e">
         <f>_xll.qlIndexFixing(FirstIndex,C7)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F7" s="14" t="str">
-        <f ca="1">IF(ISERROR(C7),_xll.ohRangeRetrieveError(C7),_xll.ohRangeRetrieveError(E7))</f>
-        <v/>
-      </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="21" t="s">
+      <c r="E7" s="13" t="str">
+        <f ca="1">IF(ISERROR(C7),_xll.ohRangeRetrieveError(C7),_xll.ohRangeRetrieveError(D7))</f>
+        <v>qlIndexFixing - Missing BBSW6M Actual/365 (Fixed) fixing for June 30th, 2014</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="22" t="str">
+      <c r="H7" s="20" t="str">
         <f>_xll.ohBoostVersion(Trigger)</f>
         <v>1_52</v>
       </c>
-      <c r="J7" s="13"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
@@ -1499,33 +1474,32 @@
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-    </row>
-    <row r="8" spans="1:23" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="39">
+      <c r="B8" s="43"/>
+      <c r="C8" s="33">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),EvaluationDate,"-1D","Preceding")</f>
-        <v>41817</v>
-      </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="26" t="e">
+        <v>41821</v>
+      </c>
+      <c r="D8" s="22" t="e">
         <f>_xll.qlIndexFixing(FirstIndex,C8)</f>
         <v>#NUM!</v>
       </c>
-      <c r="F8" s="18" t="str">
-        <f ca="1">IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(E8))</f>
-        <v/>
-      </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="21" t="s">
+      <c r="E8" s="16" t="str">
+        <f ca="1">IF(ISERROR(C8),_xll.ohRangeRetrieveError(C8),_xll.ohRangeRetrieveError(D8))</f>
+        <v>qlIndexFixing - Missing BBSW6M Actual/365 (Fixed) fixing for July 1st, 2014</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="22" t="str">
+      <c r="H8" s="20" t="str">
         <f>_xll.qlVersion(Trigger)</f>
         <v>1.5</v>
       </c>
-      <c r="J8" s="13"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
@@ -1538,33 +1512,32 @@
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-    </row>
-    <row r="9" spans="1:23" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="39">
+      <c r="B9" s="43"/>
+      <c r="C9" s="33">
         <f>EvaluationDate</f>
-        <v>41820</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26">
+        <v>41822</v>
+      </c>
+      <c r="D9" s="22">
         <f>_xll.qlIndexFixing(FirstIndex,C9)</f>
         <v>2.7250000000000031E-2</v>
       </c>
-      <c r="F9" s="18" t="str">
-        <f>IF(ISERROR(C9),_xll.ohRangeRetrieveError(C9),_xll.ohRangeRetrieveError(E9))</f>
+      <c r="E9" s="16" t="str">
+        <f>IF(ISERROR(C9),_xll.ohRangeRetrieveError(C9),_xll.ohRangeRetrieveError(D9))</f>
         <v/>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="30" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="31" t="str">
+      <c r="H9" s="26" t="str">
         <f>_xll.ohVersion(Trigger)</f>
         <v>1.5.0</v>
       </c>
-      <c r="J9" s="13"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="4"/>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
@@ -1577,28 +1550,27 @@
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-    </row>
-    <row r="10" spans="1:23" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="50"/>
-      <c r="C10" s="40">
+      <c r="B10" s="44"/>
+      <c r="C10" s="34">
         <f>_xll.qlCalendarAdvance(_xll.qlIndexFixingCalendar(FirstIndex),_xll.qlIMMNextDate(_xll.qlIMMNextDate(EvaluationDate+1)+1),-_xll.qlInterestRateIndexFixingDays(FirstIndex)&amp;"D")</f>
         <v>41990</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28">
+      <c r="D10" s="23">
         <f>_xll.qlIndexFixing(FirstIndex,C10,TRUE)</f>
-        <v>2.648475472911983E-2</v>
-      </c>
-      <c r="F10" s="29" t="str">
-        <f>IF(ISERROR(C10),_xll.ohRangeRetrieveError(C10),_xll.ohRangeRetrieveError(E10))</f>
+        <v>2.6417212935150629E-2</v>
+      </c>
+      <c r="E10" s="24" t="str">
+        <f>IF(ISERROR(C10),_xll.ohRangeRetrieveError(C10),_xll.ohRangeRetrieveError(D10))</f>
         <v/>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="13"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -1611,19 +1583,18 @@
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-    </row>
-    <row r="11" spans="1:23" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="33"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="35"/>
+    </row>
+    <row r="11" spans="1:22" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="4"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
@@ -1636,9 +1607,8 @@
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1661,9 +1631,8 @@
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
       <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1686,9 +1655,8 @@
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1711,9 +1679,8 @@
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1736,9 +1703,8 @@
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
       <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1761,9 +1727,8 @@
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
       <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1786,9 +1751,8 @@
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
       <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1811,9 +1775,8 @@
       <c r="T18" s="4"/>
       <c r="U18" s="4"/>
       <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1836,9 +1799,8 @@
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
       <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1861,9 +1823,8 @@
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1886,9 +1847,8 @@
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
       <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1911,9 +1871,8 @@
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1936,9 +1895,8 @@
       <c r="T23" s="4"/>
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1961,15 +1919,14 @@
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
+      <c r="F25" s="45"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
@@ -1986,9 +1943,8 @@
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2011,9 +1967,8 @@
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
-      <c r="W26" s="4"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2036,9 +1991,8 @@
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2061,9 +2015,8 @@
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
-      <c r="W28" s="4"/>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2086,9 +2039,8 @@
       <c r="T29" s="4"/>
       <c r="U29" s="4"/>
       <c r="V29" s="4"/>
-      <c r="W29" s="4"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2111,9 +2063,8 @@
       <c r="T30" s="4"/>
       <c r="U30" s="4"/>
       <c r="V30" s="4"/>
-      <c r="W30" s="4"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2136,9 +2087,8 @@
       <c r="T31" s="4"/>
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
-      <c r="W31" s="4"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2161,9 +2111,8 @@
       <c r="T32" s="4"/>
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2186,9 +2135,8 @@
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
       <c r="V33" s="4"/>
-      <c r="W33" s="4"/>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2211,9 +2159,8 @@
       <c r="T34" s="4"/>
       <c r="U34" s="4"/>
       <c r="V34" s="4"/>
-      <c r="W34" s="4"/>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2236,9 +2183,8 @@
       <c r="T35" s="4"/>
       <c r="U35" s="4"/>
       <c r="V35" s="4"/>
-      <c r="W35" s="4"/>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2261,9 +2207,8 @@
       <c r="T36" s="4"/>
       <c r="U36" s="4"/>
       <c r="V36" s="4"/>
-      <c r="W36" s="4"/>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2286,9 +2231,8 @@
       <c r="T37" s="4"/>
       <c r="U37" s="4"/>
       <c r="V37" s="4"/>
-      <c r="W37" s="4"/>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2311,9 +2255,8 @@
       <c r="T38" s="4"/>
       <c r="U38" s="4"/>
       <c r="V38" s="4"/>
-      <c r="W38" s="4"/>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2336,9 +2279,8 @@
       <c r="T39" s="4"/>
       <c r="U39" s="4"/>
       <c r="V39" s="4"/>
-      <c r="W39" s="4"/>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2361,9 +2303,8 @@
       <c r="T40" s="4"/>
       <c r="U40" s="4"/>
       <c r="V40" s="4"/>
-      <c r="W40" s="4"/>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2386,9 +2327,8 @@
       <c r="T41" s="4"/>
       <c r="U41" s="4"/>
       <c r="V41" s="4"/>
-      <c r="W41" s="4"/>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2411,9 +2351,8 @@
       <c r="T42" s="4"/>
       <c r="U42" s="4"/>
       <c r="V42" s="4"/>
-      <c r="W42" s="4"/>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2436,9 +2375,8 @@
       <c r="T43" s="4"/>
       <c r="U43" s="4"/>
       <c r="V43" s="4"/>
-      <c r="W43" s="4"/>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -2461,9 +2399,8 @@
       <c r="T44" s="4"/>
       <c r="U44" s="4"/>
       <c r="V44" s="4"/>
-      <c r="W44" s="4"/>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2486,9 +2423,8 @@
       <c r="T45" s="4"/>
       <c r="U45" s="4"/>
       <c r="V45" s="4"/>
-      <c r="W45" s="4"/>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2511,9 +2447,8 @@
       <c r="T46" s="4"/>
       <c r="U46" s="4"/>
       <c r="V46" s="4"/>
-      <c r="W46" s="4"/>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -2536,9 +2471,8 @@
       <c r="T47" s="4"/>
       <c r="U47" s="4"/>
       <c r="V47" s="4"/>
-      <c r="W47" s="4"/>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2561,9 +2495,8 @@
       <c r="T48" s="4"/>
       <c r="U48" s="4"/>
       <c r="V48" s="4"/>
-      <c r="W48" s="4"/>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -2586,9 +2519,8 @@
       <c r="T49" s="4"/>
       <c r="U49" s="4"/>
       <c r="V49" s="4"/>
-      <c r="W49" s="4"/>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -2611,9 +2543,8 @@
       <c r="T50" s="4"/>
       <c r="U50" s="4"/>
       <c r="V50" s="4"/>
-      <c r="W50" s="4"/>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2636,16 +2567,15 @@
       <c r="T51" s="4"/>
       <c r="U51" s="4"/>
       <c r="V51" s="4"/>
-      <c r="W51" s="4"/>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
+      <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
@@ -2659,10 +2589,10 @@
       <c r="T52" s="4"/>
       <c r="U52" s="4"/>
       <c r="V52" s="4"/>
-      <c r="W52" s="4"/>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" s="4"/>
+      <c r="I53" s="4"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
@@ -2676,9 +2606,9 @@
       <c r="T53" s="4"/>
       <c r="U53" s="4"/>
       <c r="V53" s="4"/>
-      <c r="W53" s="4"/>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
       <c r="M54" s="4"/>
@@ -2691,9 +2621,9 @@
       <c r="T54" s="4"/>
       <c r="U54" s="4"/>
       <c r="V54" s="4"/>
-      <c r="W54" s="4"/>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
@@ -2706,9 +2636,9 @@
       <c r="T55" s="4"/>
       <c r="U55" s="4"/>
       <c r="V55" s="4"/>
-      <c r="W55" s="4"/>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
@@ -2721,9 +2651,9 @@
       <c r="T56" s="4"/>
       <c r="U56" s="4"/>
       <c r="V56" s="4"/>
-      <c r="W56" s="4"/>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
@@ -2736,9 +2666,9 @@
       <c r="T57" s="4"/>
       <c r="U57" s="4"/>
       <c r="V57" s="4"/>
-      <c r="W57" s="4"/>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
@@ -2751,7 +2681,6 @@
       <c r="T58" s="4"/>
       <c r="U58" s="4"/>
       <c r="V58" s="4"/>
-      <c r="W58" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2771,7 +2700,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId4" name="CommandButton1">
+        <control shapeId="1026" r:id="rId4" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -2791,12 +2720,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId6" name="CommandButton2">
+        <control shapeId="1025" r:id="rId6" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -2816,7 +2745,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
MainChecks link to Market removed
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/AUD_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/AUD_MainChecks.xlsx
@@ -9,16 +9,13 @@
   <sheets>
     <sheet name="MainChecks" sheetId="2" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="Currency">MainChecks!$U$4</definedName>
-    <definedName name="FirstIndex">MainChecks!$K$11</definedName>
+    <definedName name="FirstIndex">MainChecks!$K$10</definedName>
     <definedName name="FuturesDates">MainChecks!$C$14:$C$17</definedName>
     <definedName name="FuturesTable">MainChecks!$A$4:$H$12</definedName>
     <definedName name="IMMFutures">MainChecks!$D$14:$D$17</definedName>
-    <definedName name="InterestRatesTrigger">MainChecks!$Q$8</definedName>
+    <definedName name="InterestRatesTrigger">MainChecks!#REF!</definedName>
     <definedName name="TenYearsBondFutures">MainChecks!$C$4:$C$6</definedName>
     <definedName name="Trigger">MainChecks!$U$2</definedName>
   </definedNames>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
   <si>
     <t>ObjectID</t>
   </si>
@@ -57,9 +54,6 @@
   </si>
   <si>
     <t>MarketData Checks</t>
-  </si>
-  <si>
-    <t># Mkt Updates</t>
   </si>
   <si>
     <t>Reference Date</t>
@@ -537,7 +531,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -550,12 +544,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -584,9 +572,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -620,15 +605,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="18" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -755,28 +731,28 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Updated at 12:59:58</v>
+        <v>Updated at 15:28:01</v>
         <stp/>
-        <stp>{505CA5DC-1664-45AC-BCD4-2E0BA32434C6}</stp>
-        <tr r="Q6" s="2"/>
+        <stp>{D16453F4-D590-48F6-B763-5A1325F3F918}</stp>
+        <tr r="Q7" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 12:59:57</v>
+        <v>Updated at 15:28:01</v>
         <stp/>
-        <stp>{F253EC00-6F38-4A29-BFFC-CBC015E8968A}</stp>
+        <stp>{5999A432-1A4F-49C4-82CA-076BA00A0F35}</stp>
+        <tr r="P7" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:28:07</v>
+        <stp/>
+        <stp>{1E6D0745-D6B1-4E79-BC3D-A4A668780DB7}</stp>
         <tr r="Q5" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 12:59:58</v>
+        <v>Updated at 15:28:01</v>
         <stp/>
-        <stp>{9E7251B4-D9C8-40ED-A5C4-29CA39283044}</stp>
-        <tr r="Q7" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 12:59:58</v>
-        <stp/>
-        <stp>{91B048FA-14CC-4783-A9DE-CEA56BA25690}</stp>
-        <tr r="P7" s="2"/>
+        <stp>{2ED66F23-F5D8-44AB-A945-AB0FC6E72BB0}</stp>
+        <tr r="Q6" s="2"/>
       </tp>
     </main>
   </volType>
@@ -876,56 +852,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="General Settings"/>
-      <sheetName val="BBSW"/>
-      <sheetName val="BBSWSwapForBasisCalc"/>
-      <sheetName val="OIS"/>
-      <sheetName val="MT_OIS"/>
-      <sheetName val="Deposits"/>
-      <sheetName val="FRA"/>
-      <sheetName val="Futures1M"/>
-      <sheetName val="Futures3M"/>
-      <sheetName val="FuturesHWConvAdj"/>
-      <sheetName val="Swap3M"/>
-      <sheetName val="Swap6M"/>
-      <sheetName val="BasisSwap1M3M"/>
-      <sheetName val="BasisSwap3M6M"/>
-      <sheetName val="AUD_Market"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="TriggerCounter" refersTo="='General Settings'!$D$7"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="7">
-          <cell r="D7">
-            <v>32</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1306,13 +1232,13 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
       <c r="R2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S2" s="1"/>
-      <c r="T2" s="22" t="s">
+      <c r="T2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="U2" s="21">
+      <c r="U2" s="19">
         <v>41834.510625000003</v>
       </c>
       <c r="V2" s="1"/>
@@ -1342,17 +1268,17 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="7"/>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="18"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="16"/>
       <c r="R3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -1378,52 +1304,52 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="7"/>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="20" t="s">
+      <c r="L4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="R4" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="S4" s="1"/>
-      <c r="T4" s="22" t="s">
+      <c r="T4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="U4" s="14" t="s">
-        <v>22</v>
+      <c r="U4" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
@@ -1443,57 +1369,57 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="44" t="s">
+      <c r="B5" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="44" t="s">
-        <v>51</v>
+      <c r="F5" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="38" t="s">
+        <v>50</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="30" t="s">
+      <c r="K5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="L5" s="31">
+      <c r="L5" s="28">
         <v>41890</v>
       </c>
-      <c r="M5" s="32">
-        <v>147.59</v>
-      </c>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="33" t="str">
+      <c r="M5" s="29">
+        <v>150.34</v>
+      </c>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="30" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>Updated at 12:59:57</v>
+        <v>Updated at 15:28:07</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S5" s="1"/>
-      <c r="T5" s="22" t="s">
+      <c r="T5" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="U5" s="14" t="str">
-        <f>_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
-        <v>1_52 / 1.5.0 / 1.5</v>
+      <c r="U5" s="12" t="e">
+        <f ca="1">_xll.ohBoostVersion(Trigger)&amp;" / "&amp;_xll.ohVersion(Trigger)&amp;" / "&amp;_xll.qlVersion(Trigger)</f>
+        <v>#NAME?</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -1513,57 +1439,57 @@
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="44" t="s">
-        <v>51</v>
+        <v>18</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>50</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" s="3"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="L6" s="28">
+      <c r="J6" s="21"/>
+      <c r="K6" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="25">
         <v>42166</v>
       </c>
-      <c r="M6" s="34">
-        <v>97.43</v>
-      </c>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="34"/>
-      <c r="Q6" s="35" t="str">
+      <c r="M6" s="31">
+        <v>97.350000000000009</v>
+      </c>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="32" t="str">
         <f>_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
-        <v>Updated at 12:59:58</v>
+        <v>Updated at 15:28:01</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S6" s="1"/>
-      <c r="T6" s="22" t="s">
+      <c r="T6" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="U6" s="14">
-        <f>_xll.ohRepositoryObjectCount(Trigger)</f>
-        <v>1587</v>
+      <c r="U6" s="12" t="e">
+        <f ca="1">_xll.ohRepositoryObjectCount(Trigger)</f>
+        <v>#NAME?</v>
       </c>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
@@ -1583,56 +1509,56 @@
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44" t="s">
+      <c r="E7" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="F7" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="44" t="s">
-        <v>53</v>
+      <c r="G7" s="38" t="s">
+        <v>52</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="27" t="str">
+      <c r="J7" s="21"/>
+      <c r="K7" s="24" t="str">
         <f>Currency&amp;VLOOKUP(Currency,FuturesTable,5,0)&amp;VLOOKUP(Currency,FuturesTable,6,0)&amp;"10Y"</f>
         <v>AUDSM6AB10Y</v>
       </c>
-      <c r="L7" s="28">
-        <v>41834</v>
-      </c>
-      <c r="M7" s="40" t="str">
+      <c r="L7" s="25">
+        <v>41873</v>
+      </c>
+      <c r="M7" s="34" t="str">
         <f>N7&amp;"/"&amp;O7</f>
-        <v>3.8/3.86</v>
-      </c>
-      <c r="N7" s="34">
-        <v>3.8000000000000003</v>
-      </c>
-      <c r="O7" s="34">
-        <v>3.8600000000000003</v>
-      </c>
-      <c r="P7" s="34" t="str">
+        <v>3.8025/3.8625</v>
+      </c>
+      <c r="N7" s="31">
+        <v>3.8025000000000002</v>
+      </c>
+      <c r="O7" s="31">
+        <v>3.8625000000000003</v>
+      </c>
+      <c r="P7" s="31" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>Updated at 12:59:58</v>
-      </c>
-      <c r="Q7" s="35" t="str">
+        <v>Updated at 15:28:01</v>
+      </c>
+      <c r="Q7" s="32" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>Updated at 12:59:58</v>
+        <v>Updated at 15:28:01</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -1653,45 +1579,42 @@
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="44" t="s">
-        <v>51</v>
+        <v>20</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="38" t="s">
+        <v>50</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" s="36"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
-      <c r="O8" s="37"/>
-      <c r="P8" s="37"/>
-      <c r="Q8" s="38">
-        <f>[1]!TriggerCounter</f>
-        <v>32</v>
-      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="16"/>
       <c r="R8" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
@@ -1712,42 +1635,48 @@
       <c r="AI8" s="3"/>
       <c r="AJ8" s="3"/>
     </row>
-    <row r="9" spans="1:36" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="F9" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="44" t="s">
-        <v>52</v>
+      <c r="G9" s="38" t="s">
+        <v>51</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="13"/>
+      <c r="K9" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="18" t="s">
+        <v>12</v>
+      </c>
       <c r="R9" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -1770,34 +1699,38 @@
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
+        <v>22</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
       <c r="H10" s="8"/>
       <c r="I10" s="3"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="20" t="s">
+      <c r="K10" s="22" t="str">
+        <f>PROPER(Currency)&amp;VLOOKUP(Currency,FuturesTable,8,0)&amp;VLOOKUP(Currency,FuturesTable,2,0)</f>
+        <v>AudBBSW6M</v>
+      </c>
+      <c r="L10" s="23" t="e">
+        <f ca="1">_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M10" s="33" t="e">
+        <f ca="1">_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="35" t="e">
+        <f ca="1">IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R10" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="R10" s="8" t="s">
-        <v>14</v>
       </c>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -1820,38 +1753,38 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
+        <v>23</v>
+      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
       <c r="H11" s="8"/>
       <c r="I11" s="3"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="25" t="str">
-        <f>PROPER(Currency)&amp;VLOOKUP(Currency,FuturesTable,8,0)&amp;VLOOKUP(Currency,FuturesTable,2,0)</f>
-        <v>AudBBSW6M</v>
-      </c>
-      <c r="L11" s="26" t="e">
-        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M11" s="39" t="e">
-        <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="41" t="e">
-        <f ca="1">IF(AND(ISERROR(L11),ISERROR(M11)),_xll.ohRangeRetrieveError(L11)&amp;" "&amp;_xll.ohRangeRetrieveError(M11),IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11)))</f>
+      <c r="K11" s="24" t="str">
+        <f>UPPER(Currency)&amp;"STD"</f>
+        <v>AUDSTD</v>
+      </c>
+      <c r="L11" s="25" t="e">
+        <f ca="1">_xll.qlTermStructureReferenceDate(K11,Trigger)</f>
         <v>#NAME?</v>
       </c>
+      <c r="M11" s="26" t="e">
+        <f ca="1">_xll.qlYieldTSDiscount(K11,L11)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="36" t="e">
+        <f ca="1">IF(ISERROR(L11),_xll.ohRangeRetrieveError(L11),_xll.ohRangeRetrieveError(M11))</f>
+        <v>#NAME?</v>
+      </c>
       <c r="R11" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
@@ -1873,47 +1806,47 @@
       <c r="AJ11" s="3"/>
     </row>
     <row r="12" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="47"/>
+      <c r="A12" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="44"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="F12" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>31</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="27" t="str">
-        <f>UPPER(Currency)&amp;"STD"</f>
-        <v>AUDSTD</v>
-      </c>
-      <c r="L12" s="28" t="e">
-        <f>_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M12" s="29" t="e">
-        <f>_xll.qlYieldTSDiscount(K12,L12)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="42" t="e">
+      <c r="K12" s="24" t="str">
+        <f>UPPER(Currency)&amp;"ON"</f>
+        <v>AUDON</v>
+      </c>
+      <c r="L12" s="25" t="e">
+        <f ca="1">_xll.qlTermStructureReferenceDate(K12,Trigger)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M12" s="26" t="e">
+        <f ca="1">_xll.qlYieldTSDiscount(K12,L12)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="37" t="e">
         <f ca="1">IF(ISERROR(L12),_xll.ohRangeRetrieveError(L12),_xll.ohRangeRetrieveError(M12))</f>
         <v>#NAME?</v>
       </c>
       <c r="R12" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
@@ -1945,27 +1878,27 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="27" t="str">
-        <f>UPPER(Currency)&amp;"ON"</f>
-        <v>AUDON</v>
-      </c>
-      <c r="L13" s="28" t="e">
-        <f>_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M13" s="29" t="e">
-        <f>_xll.qlYieldTSDiscount(K13,L13)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="43" t="e">
+      <c r="K13" s="24" t="str">
+        <f>UPPER(Currency)&amp;"3M"</f>
+        <v>AUD3M</v>
+      </c>
+      <c r="L13" s="25" t="e">
+        <f ca="1">_xll.qlTermStructureReferenceDate(K13,Trigger)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M13" s="26" t="e">
+        <f ca="1">_xll.qlYieldTSDiscount(K13,L13)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="37" t="e">
         <f ca="1">IF(ISERROR(L13),_xll.ohRangeRetrieveError(L13),_xll.ohRangeRetrieveError(M13))</f>
         <v>#NAME?</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
@@ -1991,13 +1924,13 @@
       <c r="B14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="C14" s="45">
-        <f t="array" ref="C14:C17">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B14:B17)</f>
-        <v>41899</v>
-      </c>
-      <c r="D14" s="6" t="str">
-        <f t="array" ref="D14:D17">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
-        <v>YBAU4</v>
+      <c r="C14" s="39" t="e">
+        <f t="array" aca="1" ref="C14:C17" ca="1">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B14:B17)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D14" s="6" t="e">
+        <f t="array" aca="1" ref="D14:D17" ca="1">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
+        <v>#NAME?</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -2005,27 +1938,27 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="27" t="str">
-        <f>UPPER(Currency)&amp;"3M"</f>
-        <v>AUD3M</v>
-      </c>
-      <c r="L14" s="28" t="e">
-        <f>_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M14" s="29" t="e">
-        <f>_xll.qlYieldTSDiscount(K14,L14)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="43" t="e">
+      <c r="K14" s="24" t="str">
+        <f>UPPER(Currency)&amp;"6M"</f>
+        <v>AUD6M</v>
+      </c>
+      <c r="L14" s="25" t="e">
+        <f ca="1">_xll.qlTermStructureReferenceDate(K14,Trigger)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M14" s="26" t="e">
+        <f ca="1">_xll.qlYieldTSDiscount(K14,L14)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="37" t="e">
         <f ca="1">IF(ISERROR(L14),_xll.ohRangeRetrieveError(L14),_xll.ohRangeRetrieveError(M14))</f>
         <v>#NAME?</v>
       </c>
       <c r="R14" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
@@ -2046,44 +1979,34 @@
       <c r="AI14" s="3"/>
       <c r="AJ14" s="3"/>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="48" t="b">
+      <c r="B15" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="C15" s="46">
-        <v>41990</v>
-      </c>
-      <c r="D15" s="8" t="str">
-        <v>YBAZ4</v>
+      <c r="C15" s="40" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D15" s="8" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="27" t="str">
-        <f>UPPER(Currency)&amp;"6M"</f>
-        <v>AUD6M</v>
-      </c>
-      <c r="L15" s="28" t="e">
-        <f>_xll.qlTermStructureReferenceDate(K15,Trigger)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M15" s="29" t="e">
-        <f>_xll.qlYieldTSDiscount(K15,L15)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N15" s="29"/>
-      <c r="O15" s="29"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="43" t="e">
-        <f ca="1">IF(ISERROR(L15),_xll.ohRangeRetrieveError(L15),_xll.ohRangeRetrieveError(M15))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="R15" s="8" t="s">
-        <v>14</v>
+      <c r="J15" s="9"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="45"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="11" t="s">
+        <v>13</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -2104,33 +2027,33 @@
       <c r="AI15" s="3"/>
       <c r="AJ15" s="3"/>
     </row>
-    <row r="16" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-      <c r="B16" s="48" t="b">
+      <c r="B16" s="42" t="b">
         <v>1</v>
       </c>
-      <c r="C16" s="46">
-        <v>42081</v>
-      </c>
-      <c r="D16" s="8" t="str">
-        <v>YBAH5</v>
+      <c r="C16" s="40" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D16" s="8" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="51"/>
-      <c r="L16" s="51"/>
-      <c r="M16" s="51"/>
-      <c r="N16" s="51"/>
-      <c r="O16" s="51"/>
-      <c r="P16" s="51"/>
-      <c r="Q16" s="51"/>
-      <c r="R16" s="11" t="s">
-        <v>14</v>
-      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
@@ -2152,14 +2075,16 @@
     </row>
     <row r="17" spans="1:36" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="49" t="b">
+      <c r="B17" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="C17" s="47">
-        <v>42172</v>
-      </c>
-      <c r="D17" s="11" t="str">
-        <v>YBAM5</v>
+      <c r="C17" s="41" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="D17" s="11" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -3048,7 +2973,7 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
-      <c r="R40" s="1"/>
+      <c r="R40" s="3"/>
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
@@ -3078,14 +3003,14 @@
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
-      <c r="N41" s="1"/>
-      <c r="O41" s="1"/>
-      <c r="P41" s="1"/>
-      <c r="Q41" s="1"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
       <c r="R41" s="3"/>
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>

</xml_diff>

<commit_message>
10Y Bond Futures in MainChecks
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/AUD_MainChecks.xlsx
+++ b/QuantLibXL/Data2/XLS/AUD_MainChecks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
   <si>
     <t>ObjectID</t>
   </si>
@@ -183,6 +183,21 @@
   </si>
   <si>
     <t>PREA</t>
+  </si>
+  <si>
+    <t>JGBc1</t>
+  </si>
+  <si>
+    <t>TRHK</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>3S</t>
+  </si>
+  <si>
+    <t>Shibor</t>
   </si>
 </sst>
 </file>
@@ -518,7 +533,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="38" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="40" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -530,8 +545,9 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -636,13 +652,16 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="10">
     <cellStyle name="Migliaia (0)_AZIONI" xfId="1"/>
     <cellStyle name="Migliaia_AZIONI" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normale_AZIONI" xfId="3"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Note 2" xfId="9"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
     <cellStyle name="result" xfId="5"/>
     <cellStyle name="Valuta (0)_AZIONI" xfId="6"/>
@@ -731,28 +750,28 @@
   <volType type="realTimeData">
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>On Pause</v>
+        <v>Updated at 17:12:59</v>
         <stp/>
-        <stp>{7B961AA7-3EB3-43DE-A9D8-B6DCF526ACC6}</stp>
+        <stp>{3F86807B-6C96-43A1-9843-D760EF82B2E1}</stp>
+        <tr r="Q6" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 17:19:32</v>
+        <stp/>
+        <stp>{858208FD-F141-4ED0-B57A-A790717C1E82}</stp>
+        <tr r="Q5" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 17:04:24</v>
+        <stp/>
+        <stp>{AE27E9C3-B4B4-45C4-A3A3-C874141F084B}</stp>
         <tr r="P7" s="2"/>
       </tp>
       <tp t="s">
-        <v>On Pause</v>
+        <v>Updated at 17:04:24</v>
         <stp/>
-        <stp>{D7CF9865-2AE6-43AD-91FA-AFA95323078F}</stp>
+        <stp>{1F1505C9-518F-4BB7-82D7-EEEDE56E41C2}</stp>
         <tr r="Q7" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>On Pause</v>
-        <stp/>
-        <stp>{4C5A8384-A89B-462A-8152-397A5B62E2F4}</stp>
-        <tr r="Q6" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>On Pause</v>
-        <stp/>
-        <stp>{0E8FCADD-17BB-4920-903B-DC702DC36F29}</stp>
-        <tr r="Q5" s="2"/>
       </tp>
     </main>
   </volType>
@@ -1155,11 +1174,11 @@
     <col min="1" max="1" width="4" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="2" max="2" width="5" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="3" max="3" width="10" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="6" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="7" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="5" max="5" width="3" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="6" max="6" width="4" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="7" max="7" width="5" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="6" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="7" style="2" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="9" max="9" width="2.7109375" style="2" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="2.7109375" style="2" customWidth="1"/>
     <col min="11" max="11" width="14.140625" style="2" bestFit="1" customWidth="1"/>
@@ -1391,21 +1410,22 @@
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="7"/>
-      <c r="K5" s="27" t="s">
-        <v>3</v>
+      <c r="K5" s="27" t="str">
+        <f>VLOOKUP(Currency,FuturesTable,3,0)</f>
+        <v>TYcm1t</v>
       </c>
       <c r="L5" s="28">
-        <v>41890</v>
+        <v>41992</v>
       </c>
       <c r="M5" s="29">
-        <v>150.92000000000002</v>
+        <v>125.796875</v>
       </c>
       <c r="N5" s="29"/>
       <c r="O5" s="29"/>
       <c r="P5" s="29"/>
       <c r="Q5" s="30" t="str">
         <f>_xll.RData(K5,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L5)</f>
-        <v>On Pause</v>
+        <v>Updated at 17:19:32</v>
       </c>
       <c r="R5" s="8" t="s">
         <v>13</v>
@@ -1468,14 +1488,14 @@
         <v>42166</v>
       </c>
       <c r="M6" s="31">
-        <v>97.350000000000009</v>
+        <v>97.28</v>
       </c>
       <c r="N6" s="31"/>
       <c r="O6" s="31"/>
       <c r="P6" s="31"/>
       <c r="Q6" s="32" t="str">
         <f>_xll.RData(K6,{"EXPIR_DATE","LAST"},,"FRQ:1S",,L6)</f>
-        <v>On Pause</v>
+        <v>Updated at 17:12:59</v>
       </c>
       <c r="R6" s="8" t="s">
         <v>13</v>
@@ -1511,7 +1531,9 @@
       <c r="B7" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="38"/>
+      <c r="C7" s="38" t="s">
+        <v>16</v>
+      </c>
       <c r="D7" s="38" t="s">
         <v>41</v>
       </c>
@@ -1534,25 +1556,25 @@
         <v>AUDSM6AB10Y</v>
       </c>
       <c r="L7" s="25">
-        <v>41876</v>
+        <v>41919</v>
       </c>
       <c r="M7" s="34" t="str">
         <f>N7&amp;"/"&amp;O7</f>
-        <v>3.77/3.83</v>
+        <v>3.7575/3.8175</v>
       </c>
       <c r="N7" s="31">
-        <v>3.77</v>
+        <v>3.7575000000000003</v>
       </c>
       <c r="O7" s="31">
-        <v>3.83</v>
+        <v>3.8175000000000003</v>
       </c>
       <c r="P7" s="31" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),{"BID","ASK"},,"FRQ:1S",,N7)</f>
-        <v>On Pause</v>
+        <v>Updated at 17:04:24</v>
       </c>
       <c r="Q7" s="32" t="str">
         <f>_xll.RData(K7&amp;"="&amp;VLOOKUP(Currency,FuturesTable,7,0),"VALUE_DT1",,"FRQ:1S",,L7)</f>
-        <v>On Pause</v>
+        <v>Updated at 17:04:24</v>
       </c>
       <c r="R7" s="8" t="s">
         <v>13</v>
@@ -1583,7 +1605,9 @@
       <c r="B8" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="38"/>
+      <c r="C8" s="38" t="s">
+        <v>53</v>
+      </c>
       <c r="D8" s="38" t="s">
         <v>44</v>
       </c>
@@ -1639,7 +1663,9 @@
       <c r="B9" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="38"/>
+      <c r="C9" s="38" t="s">
+        <v>16</v>
+      </c>
       <c r="D9" s="38" t="s">
         <v>45</v>
       </c>
@@ -1698,13 +1724,27 @@
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="8"/>
+      <c r="B10" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="46" t="s">
+        <v>57</v>
+      </c>
       <c r="I10" s="3"/>
       <c r="J10" s="7"/>
       <c r="K10" s="22" t="str">
@@ -1712,19 +1752,19 @@
         <v>AudBBSW6M</v>
       </c>
       <c r="L10" s="23" t="e">
-        <f>_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>#NUM!</v>
+        <f ca="1">_xll.qlLastFixingQuoteReferenceDate(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>#NAME?</v>
       </c>
       <c r="M10" s="33" t="e">
-        <f>_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
-        <v>#NUM!</v>
+        <f ca="1">_xll.qlQuoteValue(FirstIndex&amp;"LastFixing_Quote",Trigger)</f>
+        <v>#NAME?</v>
       </c>
       <c r="N10" s="33"/>
       <c r="O10" s="33"/>
       <c r="P10" s="33"/>
-      <c r="Q10" s="35" t="str">
+      <c r="Q10" s="35" t="e">
         <f ca="1">IF(AND(ISERROR(L10),ISERROR(M10)),_xll.ohRangeRetrieveError(L10)&amp;" "&amp;_xll.ohRangeRetrieveError(M10),IF(ISERROR(L10),_xll.ohRangeRetrieveError(L10),_xll.ohRangeRetrieveError(M10)))</f>
-        <v>qlLastFixingQuoteReferenceDate - empty timeseries qlQuoteValue - BBSW6M Actual/365 (Fixed) has no fixing</v>
+        <v>#NAME?</v>
       </c>
       <c r="R10" s="8" t="s">
         <v>13</v>
@@ -1752,13 +1792,27 @@
       <c r="A11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="8"/>
+      <c r="B11" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="H11" s="46" t="s">
+        <v>37</v>
+      </c>
       <c r="I11" s="3"/>
       <c r="J11" s="7"/>
       <c r="K11" s="24" t="str">
@@ -1925,9 +1979,9 @@
         <f t="array" ref="C14:C17">_xll.qlIMMNextDates(_xll.qlSettingsEvaluationDate(Trigger)-1,B14:B17)</f>
         <v>41899</v>
       </c>
-      <c r="D14" s="6" t="str">
-        <f t="array" ref="D14:D17">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
-        <v>YBAU4</v>
+      <c r="D14" s="6" t="e">
+        <f t="array" aca="1" ref="D14:D17" ca="1">VLOOKUP(Currency,FuturesTable,4,0)&amp;_xll.qlIMMcode(FuturesDates)</f>
+        <v>#NAME?</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1984,8 +2038,9 @@
       <c r="C15" s="40">
         <v>41990</v>
       </c>
-      <c r="D15" s="8" t="str">
-        <v>YBAZ4</v>
+      <c r="D15" s="8" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -2042,8 +2097,9 @@
       <c r="C16" s="40">
         <v>42081</v>
       </c>
-      <c r="D16" s="8" t="str">
-        <v>YBAH5</v>
+      <c r="D16" s="8" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2088,8 +2144,9 @@
       <c r="C17" s="41">
         <v>42172</v>
       </c>
-      <c r="D17" s="11" t="str">
-        <v>YBAM5</v>
+      <c r="D17" s="11" t="e">
+        <f ca="1"/>
+        <v>#NAME?</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -5291,12 +5348,9 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U4">
       <formula1>"EUR,USD,GBP,JPY,CHF,AUD,CNY,CNH,HKD"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5">
-      <formula1>TenYearsBondFutures</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6">
       <formula1>IMMFutures</formula1>
@@ -5310,7 +5364,7 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="CommandButton2">
+        <control shapeId="1025" r:id="rId4" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5330,12 +5384,12 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="CommandButton2"/>
+        <control shapeId="1025" r:id="rId4" name="CommandButton1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId6" name="CommandButton1">
+        <control shapeId="1026" r:id="rId6" name="CommandButton2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
@@ -5355,7 +5409,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId6" name="CommandButton1"/>
+        <control shapeId="1026" r:id="rId6" name="CommandButton2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>